<commit_message>
Added some additional features.
</commit_message>
<xml_diff>
--- a/xlsx/with-data.xlsx
+++ b/xlsx/with-data.xlsx
@@ -8,6 +8,9 @@
   <sheets>
     <sheet name="TAB_NAME" r:id="rId3" sheetId="1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">TAB_NAME!$A$1:$E$101</definedName>
+  </definedNames>
 </workbook>
 </file>
 
@@ -1392,7 +1395,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:F101"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="true"/>
+    <sheetView workbookViewId="0" tabSelected="true" zoomScale="150"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
@@ -3121,6 +3124,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E101"/>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added example of reading xlsx file. Added config for JUL.
</commit_message>
<xml_diff>
--- a/xlsx/with-data.xlsx
+++ b/xlsx/with-data.xlsx
@@ -6,10 +6,10 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="TAB_NAME" r:id="rId3" sheetId="1"/>
+    <sheet name="TAB NAME" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">TAB_NAME!$A$1:$E$101</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">'TAB NAME'!$A$1:$E$101</definedName>
   </definedNames>
 </workbook>
 </file>

</xml_diff>

<commit_message>
Added completed example of reading xlsx file with data. Refactoring.
</commit_message>
<xml_diff>
--- a/xlsx/with-data.xlsx
+++ b/xlsx/with-data.xlsx
@@ -1437,7 +1437,7 @@
         <v>8</v>
       </c>
       <c r="E2" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="3">
@@ -1454,7 +1454,7 @@
         <v>12</v>
       </c>
       <c r="E3" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="4">
@@ -1471,7 +1471,7 @@
         <v>16</v>
       </c>
       <c r="E4" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="5">
@@ -1488,7 +1488,7 @@
         <v>20</v>
       </c>
       <c r="E5" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="6">
@@ -1505,7 +1505,7 @@
         <v>24</v>
       </c>
       <c r="E6" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="7">
@@ -1522,7 +1522,7 @@
         <v>28</v>
       </c>
       <c r="E7" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="8">
@@ -1539,7 +1539,7 @@
         <v>32</v>
       </c>
       <c r="E8" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="9">
@@ -1556,7 +1556,7 @@
         <v>36</v>
       </c>
       <c r="E9" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="10">
@@ -1573,7 +1573,7 @@
         <v>40</v>
       </c>
       <c r="E10" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="11">
@@ -1590,7 +1590,7 @@
         <v>44</v>
       </c>
       <c r="E11" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="12">
@@ -1607,7 +1607,7 @@
         <v>48</v>
       </c>
       <c r="E12" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>10.0</v>
       </c>
     </row>
     <row r="13">
@@ -1624,7 +1624,7 @@
         <v>52</v>
       </c>
       <c r="E13" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>11.0</v>
       </c>
     </row>
     <row r="14">
@@ -1641,7 +1641,7 @@
         <v>56</v>
       </c>
       <c r="E14" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>12.0</v>
       </c>
     </row>
     <row r="15">
@@ -1658,7 +1658,7 @@
         <v>60</v>
       </c>
       <c r="E15" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>13.0</v>
       </c>
     </row>
     <row r="16">
@@ -1675,7 +1675,7 @@
         <v>64</v>
       </c>
       <c r="E16" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>14.0</v>
       </c>
     </row>
     <row r="17">
@@ -1692,7 +1692,7 @@
         <v>68</v>
       </c>
       <c r="E17" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>15.0</v>
       </c>
     </row>
     <row r="18">
@@ -1709,7 +1709,7 @@
         <v>72</v>
       </c>
       <c r="E18" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>16.0</v>
       </c>
     </row>
     <row r="19">
@@ -1726,7 +1726,7 @@
         <v>76</v>
       </c>
       <c r="E19" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>17.0</v>
       </c>
     </row>
     <row r="20">
@@ -1743,7 +1743,7 @@
         <v>80</v>
       </c>
       <c r="E20" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>18.0</v>
       </c>
     </row>
     <row r="21">
@@ -1760,7 +1760,7 @@
         <v>84</v>
       </c>
       <c r="E21" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>19.0</v>
       </c>
     </row>
     <row r="22">
@@ -1777,7 +1777,7 @@
         <v>88</v>
       </c>
       <c r="E22" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>20.0</v>
       </c>
     </row>
     <row r="23">
@@ -1794,7 +1794,7 @@
         <v>92</v>
       </c>
       <c r="E23" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>21.0</v>
       </c>
     </row>
     <row r="24">
@@ -1811,7 +1811,7 @@
         <v>96</v>
       </c>
       <c r="E24" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>22.0</v>
       </c>
     </row>
     <row r="25">
@@ -1828,7 +1828,7 @@
         <v>100</v>
       </c>
       <c r="E25" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>23.0</v>
       </c>
     </row>
     <row r="26">
@@ -1845,7 +1845,7 @@
         <v>104</v>
       </c>
       <c r="E26" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>24.0</v>
       </c>
     </row>
     <row r="27">
@@ -1862,7 +1862,7 @@
         <v>108</v>
       </c>
       <c r="E27" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>25.0</v>
       </c>
     </row>
     <row r="28">
@@ -1879,7 +1879,7 @@
         <v>112</v>
       </c>
       <c r="E28" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>26.0</v>
       </c>
     </row>
     <row r="29">
@@ -1896,7 +1896,7 @@
         <v>116</v>
       </c>
       <c r="E29" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>27.0</v>
       </c>
     </row>
     <row r="30">
@@ -1913,7 +1913,7 @@
         <v>120</v>
       </c>
       <c r="E30" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>28.0</v>
       </c>
     </row>
     <row r="31">
@@ -1930,7 +1930,7 @@
         <v>124</v>
       </c>
       <c r="E31" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>29.0</v>
       </c>
     </row>
     <row r="32">
@@ -1947,7 +1947,7 @@
         <v>128</v>
       </c>
       <c r="E32" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>30.0</v>
       </c>
     </row>
     <row r="33">
@@ -1964,7 +1964,7 @@
         <v>132</v>
       </c>
       <c r="E33" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>31.0</v>
       </c>
     </row>
     <row r="34">
@@ -1981,7 +1981,7 @@
         <v>136</v>
       </c>
       <c r="E34" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>32.0</v>
       </c>
     </row>
     <row r="35">
@@ -1998,7 +1998,7 @@
         <v>140</v>
       </c>
       <c r="E35" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>33.0</v>
       </c>
     </row>
     <row r="36">
@@ -2015,7 +2015,7 @@
         <v>144</v>
       </c>
       <c r="E36" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>34.0</v>
       </c>
     </row>
     <row r="37">
@@ -2032,7 +2032,7 @@
         <v>148</v>
       </c>
       <c r="E37" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>35.0</v>
       </c>
     </row>
     <row r="38">
@@ -2049,7 +2049,7 @@
         <v>152</v>
       </c>
       <c r="E38" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>36.0</v>
       </c>
     </row>
     <row r="39">
@@ -2066,7 +2066,7 @@
         <v>156</v>
       </c>
       <c r="E39" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>37.0</v>
       </c>
     </row>
     <row r="40">
@@ -2083,7 +2083,7 @@
         <v>160</v>
       </c>
       <c r="E40" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>38.0</v>
       </c>
     </row>
     <row r="41">
@@ -2100,7 +2100,7 @@
         <v>164</v>
       </c>
       <c r="E41" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>39.0</v>
       </c>
     </row>
     <row r="42">
@@ -2117,7 +2117,7 @@
         <v>168</v>
       </c>
       <c r="E42" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>40.0</v>
       </c>
     </row>
     <row r="43">
@@ -2134,7 +2134,7 @@
         <v>172</v>
       </c>
       <c r="E43" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>41.0</v>
       </c>
     </row>
     <row r="44">
@@ -2151,7 +2151,7 @@
         <v>176</v>
       </c>
       <c r="E44" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>42.0</v>
       </c>
     </row>
     <row r="45">
@@ -2168,7 +2168,7 @@
         <v>180</v>
       </c>
       <c r="E45" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>43.0</v>
       </c>
     </row>
     <row r="46">
@@ -2185,7 +2185,7 @@
         <v>184</v>
       </c>
       <c r="E46" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>44.0</v>
       </c>
     </row>
     <row r="47">
@@ -2202,7 +2202,7 @@
         <v>188</v>
       </c>
       <c r="E47" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>45.0</v>
       </c>
     </row>
     <row r="48">
@@ -2219,7 +2219,7 @@
         <v>192</v>
       </c>
       <c r="E48" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>46.0</v>
       </c>
     </row>
     <row r="49">
@@ -2236,7 +2236,7 @@
         <v>196</v>
       </c>
       <c r="E49" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>47.0</v>
       </c>
     </row>
     <row r="50">
@@ -2253,7 +2253,7 @@
         <v>200</v>
       </c>
       <c r="E50" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>48.0</v>
       </c>
     </row>
     <row r="51">
@@ -2270,7 +2270,7 @@
         <v>204</v>
       </c>
       <c r="E51" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>49.0</v>
       </c>
     </row>
     <row r="52">
@@ -2287,7 +2287,7 @@
         <v>208</v>
       </c>
       <c r="E52" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>50.0</v>
       </c>
     </row>
     <row r="53">
@@ -2304,7 +2304,7 @@
         <v>212</v>
       </c>
       <c r="E53" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>51.0</v>
       </c>
     </row>
     <row r="54">
@@ -2321,7 +2321,7 @@
         <v>216</v>
       </c>
       <c r="E54" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>52.0</v>
       </c>
     </row>
     <row r="55">
@@ -2338,7 +2338,7 @@
         <v>220</v>
       </c>
       <c r="E55" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>53.0</v>
       </c>
     </row>
     <row r="56">
@@ -2355,7 +2355,7 @@
         <v>224</v>
       </c>
       <c r="E56" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>54.0</v>
       </c>
     </row>
     <row r="57">
@@ -2372,7 +2372,7 @@
         <v>228</v>
       </c>
       <c r="E57" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>55.0</v>
       </c>
     </row>
     <row r="58">
@@ -2389,7 +2389,7 @@
         <v>232</v>
       </c>
       <c r="E58" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>56.0</v>
       </c>
     </row>
     <row r="59">
@@ -2406,7 +2406,7 @@
         <v>236</v>
       </c>
       <c r="E59" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>57.0</v>
       </c>
     </row>
     <row r="60">
@@ -2423,7 +2423,7 @@
         <v>240</v>
       </c>
       <c r="E60" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>58.0</v>
       </c>
     </row>
     <row r="61">
@@ -2440,7 +2440,7 @@
         <v>244</v>
       </c>
       <c r="E61" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>59.0</v>
       </c>
     </row>
     <row r="62">
@@ -2457,7 +2457,7 @@
         <v>248</v>
       </c>
       <c r="E62" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>60.0</v>
       </c>
     </row>
     <row r="63">
@@ -2474,7 +2474,7 @@
         <v>252</v>
       </c>
       <c r="E63" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>61.0</v>
       </c>
     </row>
     <row r="64">
@@ -2491,7 +2491,7 @@
         <v>256</v>
       </c>
       <c r="E64" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>62.0</v>
       </c>
     </row>
     <row r="65">
@@ -2508,7 +2508,7 @@
         <v>260</v>
       </c>
       <c r="E65" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>63.0</v>
       </c>
     </row>
     <row r="66">
@@ -2525,7 +2525,7 @@
         <v>264</v>
       </c>
       <c r="E66" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>64.0</v>
       </c>
     </row>
     <row r="67">
@@ -2542,7 +2542,7 @@
         <v>268</v>
       </c>
       <c r="E67" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>65.0</v>
       </c>
     </row>
     <row r="68">
@@ -2559,7 +2559,7 @@
         <v>272</v>
       </c>
       <c r="E68" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>66.0</v>
       </c>
     </row>
     <row r="69">
@@ -2576,7 +2576,7 @@
         <v>276</v>
       </c>
       <c r="E69" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>67.0</v>
       </c>
     </row>
     <row r="70">
@@ -2593,7 +2593,7 @@
         <v>280</v>
       </c>
       <c r="E70" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>68.0</v>
       </c>
     </row>
     <row r="71">
@@ -2610,7 +2610,7 @@
         <v>284</v>
       </c>
       <c r="E71" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>69.0</v>
       </c>
     </row>
     <row r="72">
@@ -2627,7 +2627,7 @@
         <v>288</v>
       </c>
       <c r="E72" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>70.0</v>
       </c>
     </row>
     <row r="73">
@@ -2644,7 +2644,7 @@
         <v>292</v>
       </c>
       <c r="E73" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>71.0</v>
       </c>
     </row>
     <row r="74">
@@ -2661,7 +2661,7 @@
         <v>296</v>
       </c>
       <c r="E74" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>72.0</v>
       </c>
     </row>
     <row r="75">
@@ -2678,7 +2678,7 @@
         <v>300</v>
       </c>
       <c r="E75" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>73.0</v>
       </c>
     </row>
     <row r="76">
@@ -2695,7 +2695,7 @@
         <v>304</v>
       </c>
       <c r="E76" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>74.0</v>
       </c>
     </row>
     <row r="77">
@@ -2712,7 +2712,7 @@
         <v>308</v>
       </c>
       <c r="E77" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>75.0</v>
       </c>
     </row>
     <row r="78">
@@ -2729,7 +2729,7 @@
         <v>312</v>
       </c>
       <c r="E78" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>76.0</v>
       </c>
     </row>
     <row r="79">
@@ -2746,7 +2746,7 @@
         <v>316</v>
       </c>
       <c r="E79" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>77.0</v>
       </c>
     </row>
     <row r="80">
@@ -2763,7 +2763,7 @@
         <v>320</v>
       </c>
       <c r="E80" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>78.0</v>
       </c>
     </row>
     <row r="81">
@@ -2780,7 +2780,7 @@
         <v>324</v>
       </c>
       <c r="E81" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>79.0</v>
       </c>
     </row>
     <row r="82">
@@ -2797,7 +2797,7 @@
         <v>328</v>
       </c>
       <c r="E82" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>80.0</v>
       </c>
     </row>
     <row r="83">
@@ -2814,7 +2814,7 @@
         <v>332</v>
       </c>
       <c r="E83" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>81.0</v>
       </c>
     </row>
     <row r="84">
@@ -2831,7 +2831,7 @@
         <v>336</v>
       </c>
       <c r="E84" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>82.0</v>
       </c>
     </row>
     <row r="85">
@@ -2848,7 +2848,7 @@
         <v>340</v>
       </c>
       <c r="E85" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>83.0</v>
       </c>
     </row>
     <row r="86">
@@ -2865,7 +2865,7 @@
         <v>344</v>
       </c>
       <c r="E86" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>84.0</v>
       </c>
     </row>
     <row r="87">
@@ -2882,7 +2882,7 @@
         <v>348</v>
       </c>
       <c r="E87" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>85.0</v>
       </c>
     </row>
     <row r="88">
@@ -2899,7 +2899,7 @@
         <v>352</v>
       </c>
       <c r="E88" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>86.0</v>
       </c>
     </row>
     <row r="89">
@@ -2916,7 +2916,7 @@
         <v>356</v>
       </c>
       <c r="E89" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>87.0</v>
       </c>
     </row>
     <row r="90">
@@ -2933,7 +2933,7 @@
         <v>360</v>
       </c>
       <c r="E90" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>88.0</v>
       </c>
     </row>
     <row r="91">
@@ -2950,7 +2950,7 @@
         <v>364</v>
       </c>
       <c r="E91" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>89.0</v>
       </c>
     </row>
     <row r="92">
@@ -2967,7 +2967,7 @@
         <v>368</v>
       </c>
       <c r="E92" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>90.0</v>
       </c>
     </row>
     <row r="93">
@@ -2984,7 +2984,7 @@
         <v>372</v>
       </c>
       <c r="E93" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>91.0</v>
       </c>
     </row>
     <row r="94">
@@ -3001,7 +3001,7 @@
         <v>376</v>
       </c>
       <c r="E94" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>92.0</v>
       </c>
     </row>
     <row r="95">
@@ -3018,7 +3018,7 @@
         <v>380</v>
       </c>
       <c r="E95" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>93.0</v>
       </c>
     </row>
     <row r="96">
@@ -3035,7 +3035,7 @@
         <v>384</v>
       </c>
       <c r="E96" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>94.0</v>
       </c>
     </row>
     <row r="97">
@@ -3052,7 +3052,7 @@
         <v>388</v>
       </c>
       <c r="E97" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>95.0</v>
       </c>
     </row>
     <row r="98">
@@ -3069,7 +3069,7 @@
         <v>392</v>
       </c>
       <c r="E98" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>96.0</v>
       </c>
     </row>
     <row r="99">
@@ -3086,7 +3086,7 @@
         <v>396</v>
       </c>
       <c r="E99" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>97.0</v>
       </c>
     </row>
     <row r="100">
@@ -3103,7 +3103,7 @@
         <v>400</v>
       </c>
       <c r="E100" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>98.0</v>
       </c>
     </row>
     <row r="101">
@@ -3120,7 +3120,7 @@
         <v>404</v>
       </c>
       <c r="E101" t="n" s="2">
-        <v>1.100000023841858</v>
+        <v>99.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>